<commit_message>
Presentacion para el ProductOwner
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>QF13001</t>
   </si>
@@ -61,6 +61,66 @@
   </si>
   <si>
     <t>matricula</t>
+  </si>
+  <si>
+    <t>LC13004</t>
+  </si>
+  <si>
+    <t>Lobos</t>
+  </si>
+  <si>
+    <t>Bryan</t>
+  </si>
+  <si>
+    <t>7.76</t>
+  </si>
+  <si>
+    <t>7.52</t>
+  </si>
+  <si>
+    <t>SR11038</t>
+  </si>
+  <si>
+    <t>AM11098</t>
+  </si>
+  <si>
+    <t>BV13003</t>
+  </si>
+  <si>
+    <t>Rodrigo</t>
+  </si>
+  <si>
+    <t>Segovia</t>
+  </si>
+  <si>
+    <t>Motto</t>
+  </si>
+  <si>
+    <t>Dario</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>Barrera</t>
+  </si>
+  <si>
+    <t>LL13002</t>
+  </si>
+  <si>
+    <t>Alam</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>8.3</t>
   </si>
 </sst>
 </file>
@@ -436,9 +496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="208" zoomScaleNormal="208" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="208" zoomScaleNormal="208" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -507,6 +569,151 @@
         <v>7</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>2013</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>2011</v>
+      </c>
+      <c r="H4">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>33</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>2011</v>
+      </c>
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>32</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6">
+        <v>2013</v>
+      </c>
+      <c r="H6">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>32</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7">
+        <v>2013</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rama antes del merge de Lobos
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\systemiqa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodri\Desktop\Rodrigo\UES\Quimica\systemiqa\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>QF13001</t>
   </si>
@@ -61,12 +61,18 @@
   </si>
   <si>
     <t>matricula</t>
+  </si>
+  <si>
+    <t>QF13002</t>
+  </si>
+  <si>
+    <t>Fuentes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,25 +412,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -453,7 +459,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -479,6 +485,35 @@
         <v>7</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>7.5</v>
+      </c>
+      <c r="G3">
+        <v>2013</v>
+      </c>
+      <c r="H3">
+        <v>7</v>
+      </c>
+      <c r="I3">
         <v>1</v>
       </c>
     </row>
@@ -495,7 +530,7 @@
       <selection activeCell="A2" sqref="A2:H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>